<commit_message>
added updated data and plots
</commit_message>
<xml_diff>
--- a/data/CLEANED- Delinquency.xlsx
+++ b/data/CLEANED- Delinquency.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haileyburk/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dmattie/Documents/projects/bsad482/termprojects/hailey/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{053EF050-5BBF-774E-AE32-1A50E4F2C390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B94F9638-3E1B-B64C-8023-1A9BB20798CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="740" windowWidth="19120" windowHeight="15140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Date</t>
   </si>
@@ -29,30 +29,6 @@
   </si>
   <si>
     <t>Toronto</t>
-  </si>
-  <si>
-    <t>2020Q2</t>
-  </si>
-  <si>
-    <t>Q3</t>
-  </si>
-  <si>
-    <t>Q4</t>
-  </si>
-  <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>2021Q2</t>
-  </si>
-  <si>
-    <t>2022Q2</t>
-  </si>
-  <si>
-    <t>2023Q2</t>
-  </si>
-  <si>
-    <t>2024Q2</t>
   </si>
   <si>
     <t>Source: Equifax and CMHC calculations</t>
@@ -117,11 +93,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,11 +405,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" zoomScale="128" zoomScaleNormal="128" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -446,8 +426,8 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>3</v>
+      <c r="A2" s="2">
+        <v>43922</v>
       </c>
       <c r="B2">
         <v>0.28000000000000003</v>
@@ -457,8 +437,8 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
+      <c r="A3" s="2">
+        <v>44013</v>
       </c>
       <c r="B3">
         <v>0.28000000000000003</v>
@@ -468,8 +448,8 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
+      <c r="A4" s="2">
+        <v>44105</v>
       </c>
       <c r="B4">
         <v>0.24</v>
@@ -479,8 +459,8 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>6</v>
+      <c r="A5" s="2">
+        <v>43831</v>
       </c>
       <c r="B5">
         <v>0.24</v>
@@ -490,8 +470,8 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>7</v>
+      <c r="A6" s="2">
+        <v>44287</v>
       </c>
       <c r="B6">
         <v>0.21</v>
@@ -501,8 +481,8 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>4</v>
+      <c r="A7" s="2">
+        <v>44378</v>
       </c>
       <c r="B7">
         <v>0.19</v>
@@ -512,8 +492,8 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>5</v>
+      <c r="A8" s="2">
+        <v>44470</v>
       </c>
       <c r="B8">
         <v>0.18</v>
@@ -523,8 +503,8 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>6</v>
+      <c r="A9" s="2">
+        <v>44197</v>
       </c>
       <c r="B9">
         <v>0.17</v>
@@ -534,8 +514,8 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>8</v>
+      <c r="A10" s="2">
+        <v>44652</v>
       </c>
       <c r="B10">
         <v>0.15</v>
@@ -545,8 +525,8 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>4</v>
+      <c r="A11" s="2">
+        <v>44743</v>
       </c>
       <c r="B11">
         <v>0.15</v>
@@ -556,8 +536,8 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>5</v>
+      <c r="A12" s="2">
+        <v>44835</v>
       </c>
       <c r="B12">
         <v>0.14000000000000001</v>
@@ -567,8 +547,8 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>6</v>
+      <c r="A13" s="2">
+        <v>44562</v>
       </c>
       <c r="B13">
         <v>0.15</v>
@@ -578,8 +558,8 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>9</v>
+      <c r="A14" s="2">
+        <v>45017</v>
       </c>
       <c r="B14">
         <v>0.15</v>
@@ -589,8 +569,8 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>4</v>
+      <c r="A15" s="2">
+        <v>45108</v>
       </c>
       <c r="B15">
         <v>0.16</v>
@@ -600,8 +580,8 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>5</v>
+      <c r="A16" s="2">
+        <v>45200</v>
       </c>
       <c r="B16">
         <v>0.17</v>
@@ -611,8 +591,8 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>6</v>
+      <c r="A17" s="2">
+        <v>44927</v>
       </c>
       <c r="B17">
         <v>0.18</v>
@@ -622,8 +602,8 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>10</v>
+      <c r="A18" s="2">
+        <v>45292</v>
       </c>
       <c r="B18">
         <v>0.2</v>
@@ -634,12 +614,12 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>